<commit_message>
Edit plots, add natural sequence analysis, and add multiDMS analysis
</commit_message>
<xml_diff>
--- a/non-pipeline_analyses/titers_and_neuts/data/042922_titer_calculations.xlsx
+++ b/non-pipeline_analyses/titers_and_neuts/data/042922_titer_calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\computational_notebooks\ccarr\2023\LASV_Josiah_GP_DMS\library_design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/bloom_j/computational_notebooks/ccarr/2023/LASV_Josiah_GP_DMS/non-pipeline_analyses/titers_and_neuts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400A86FE-8CB3-498A-99BA-099DB2FAA607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24ED116A-D7D7-C345-BCA5-721D39E60822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2775" yWindow="3735" windowWidth="21600" windowHeight="11295" xr2:uid="{43F769C3-2539-481E-B654-5C9B5F3B3549}"/>
+    <workbookView xWindow="11880" yWindow="4660" windowWidth="21600" windowHeight="11300" xr2:uid="{43F769C3-2539-481E-B654-5C9B5F3B3549}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -115,9 +115,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,19 +434,19 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,9 +463,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>0.69</v>
@@ -477,14 +476,13 @@
       <c r="D2">
         <v>1E-3</v>
       </c>
-      <c r="E2" s="1">
-        <f>-LN(1-B2/100)*(C2)/(D2)</f>
+      <c r="E2">
         <v>186945.70696625335</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>0.69</v>
@@ -495,17 +493,16 @@
       <c r="D3">
         <v>1E-3</v>
       </c>
-      <c r="E3" s="1">
-        <f t="shared" ref="E3:E9" si="0">-LN(1-B3/100)*(C3)/(D3)</f>
+      <c r="E3">
         <v>186945.70696625335</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>0.23</v>
+        <v>0.31</v>
       </c>
       <c r="C4">
         <v>27000</v>
@@ -513,17 +510,16 @@
       <c r="D4">
         <v>0.01</v>
       </c>
-      <c r="E4" s="1">
-        <f t="shared" si="0"/>
-        <v>6217.1524692240064</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>8383.0003743926427</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>0.31</v>
+        <v>0.23</v>
       </c>
       <c r="C5">
         <v>27000</v>
@@ -531,17 +527,16 @@
       <c r="D5">
         <v>0.01</v>
       </c>
-      <c r="E5" s="1">
-        <f t="shared" si="0"/>
-        <v>8383.0003743926427</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>6217.1524692240064</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>3.23</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="C6">
         <v>27000</v>
@@ -549,17 +544,16 @@
       <c r="D6">
         <v>1E-3</v>
       </c>
-      <c r="E6" s="1">
-        <f t="shared" si="0"/>
-        <v>886495.24157148576</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>675274.40111252945</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>2.4700000000000002</v>
+        <v>3.23</v>
       </c>
       <c r="C7">
         <v>27000</v>
@@ -567,17 +561,16 @@
       <c r="D7">
         <v>1E-3</v>
       </c>
-      <c r="E7" s="1">
-        <f t="shared" si="0"/>
-        <v>675274.40111252945</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>886495.24157148576</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8">
-        <v>9.4200000000000002E-4</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>27000</v>
@@ -585,17 +578,16 @@
       <c r="D8">
         <v>0.1</v>
       </c>
-      <c r="E8" s="1">
-        <f t="shared" si="0"/>
-        <v>2.5434119794994183</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>9.4200000000000002E-4</v>
       </c>
       <c r="C9">
         <v>27000</v>
@@ -603,9 +595,8 @@
       <c r="D9">
         <v>0.1</v>
       </c>
-      <c r="E9" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="E9">
+        <v>2.5434119794994183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>